<commit_message>
added the normalization stuff eg,NF tables and NF1,NF2, NF3
</commit_message>
<xml_diff>
--- a/Assessement1_itteration1/NormilazationTables/NF_1.xlsx
+++ b/Assessement1_itteration1/NormilazationTables/NF_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a8d0d7d0752df86/Documents/GitHub/BCDE103/Assessement1_itteration1/NormilazationTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="594" documentId="8_{1428531A-2172-4493-84B4-CAD89535E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F5F4965-FC62-4986-82B9-F4B03640A390}"/>
+  <xr:revisionPtr revIDLastSave="600" documentId="8_{1428531A-2172-4493-84B4-CAD89535E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AE58B89-CE74-4A6B-A60E-2BF0FFA59D9B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19350" yWindow="4035" windowWidth="27135" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -2519,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B101"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>